<commit_message>
OnlineController 작성 및 개인 worksheet작성
</commit_message>
<xml_diff>
--- a/documents/IndividualWorkSheet_Team1.xlsx
+++ b/documents/IndividualWorkSheet_Team1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="101">
   <si>
     <t>할일</t>
   </si>
@@ -561,6 +561,102 @@
         <charset val="129"/>
       </rPr>
       <t>에서 send, receive제대로 작동하는지 확인해야함</t>
+    </r>
+  </si>
+  <si>
+    <t>OnlineController 작성</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">connection </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>객체</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>넘겨받는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>부분</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>필요함</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>connection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">과 연동하여 작동하는 부분 작성 </t>
     </r>
   </si>
 </sst>
@@ -577,6 +673,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1142,7 +1239,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1845,7 +1942,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2028,13 +2125,25 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+    <row r="10" spans="1:6" ht="75">
+      <c r="A10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2">
+        <v>42153</v>
+      </c>
+      <c r="D10" s="2">
+        <v>42153</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
Schedule table 최신화된 버전 commit, 개인 worksheet작성
</commit_message>
<xml_diff>
--- a/documents/IndividualWorkSheet_Team1.xlsx
+++ b/documents/IndividualWorkSheet_Team1.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\RhythmCatchball\documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9824F7DE-35F2-40D1-ACC8-AEEBA93FC8C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="김민종" sheetId="5" r:id="rId1"/>
@@ -20,18 +14,18 @@
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
   <si>
     <t>할일</t>
   </si>
@@ -590,7 +584,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -611,7 +605,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -632,7 +626,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -680,27 +674,69 @@
   <si>
     <t>switch에 default없어서 경고뜬거 없앰</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code refactoring</t>
+  </si>
+  <si>
+    <t>schedule table update</t>
+  </si>
+  <si>
+    <t>일정 현황 밑 계획 최신화</t>
+  </si>
+  <si>
+    <t>SonarQube 분석 및 code smell수정</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">blank method </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>주석처리, GameSprite 파일 처리 미완된 부분 처리, UpdateGame 메소드이름 변경</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>jpeg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="굴림"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일로 만들어 git에 docments 폴더에 커밋</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -721,15 +757,33 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -772,15 +826,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -792,15 +852,21 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -812,11 +878,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -836,11 +902,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -860,11 +926,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -884,11 +950,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -913,60 +979,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table146" displayName="Table146" ref="A1:F15" totalsRowShown="0">
-  <autoFilter ref="A1:F15" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="A1:F15" totalsRowShown="0">
+  <autoFilter ref="A1:F15"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="할일" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="내용" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="할당일" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="완성일" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="결과" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="문제점" dataDxfId="18"/>
+    <tableColumn id="1" name="할일" dataDxfId="23"/>
+    <tableColumn id="2" name="내용" dataDxfId="22"/>
+    <tableColumn id="3" name="할당일" dataDxfId="21"/>
+    <tableColumn id="4" name="완성일" dataDxfId="20"/>
+    <tableColumn id="5" name="결과" dataDxfId="19"/>
+    <tableColumn id="6" name="문제점" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1467" displayName="Table1467" ref="A1:F15" totalsRowShown="0">
-  <autoFilter ref="A1:F15" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1467" displayName="Table1467" ref="A1:F15" totalsRowShown="0">
+  <autoFilter ref="A1:F15"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="할일" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="내용" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="할당일" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="완성일" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="결과" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="문제점" dataDxfId="12"/>
+    <tableColumn id="1" name="할일" dataDxfId="17"/>
+    <tableColumn id="2" name="내용" dataDxfId="16"/>
+    <tableColumn id="3" name="할당일" dataDxfId="15"/>
+    <tableColumn id="4" name="완성일" dataDxfId="14"/>
+    <tableColumn id="5" name="결과" dataDxfId="13"/>
+    <tableColumn id="6" name="문제점" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:F15" totalsRowShown="0">
-  <autoFilter ref="A1:F15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:F15" totalsRowShown="0">
+  <autoFilter ref="A1:F15"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="할일" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="내용" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="할당일" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="완성일" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="결과" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="문제점" dataDxfId="6"/>
+    <tableColumn id="1" name="할일" dataDxfId="11"/>
+    <tableColumn id="2" name="내용" dataDxfId="10"/>
+    <tableColumn id="3" name="할당일" dataDxfId="9"/>
+    <tableColumn id="4" name="완성일" dataDxfId="8"/>
+    <tableColumn id="5" name="결과" dataDxfId="7"/>
+    <tableColumn id="6" name="문제점" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table15" displayName="Table15" ref="A1:F15" totalsRowShown="0">
-  <autoFilter ref="A1:F15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:F15" totalsRowShown="0">
+  <autoFilter ref="A1:F15"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="할일" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="내용" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="할당일" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="완성일" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="결과" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="문제점" dataDxfId="0"/>
+    <tableColumn id="1" name="할일" dataDxfId="5"/>
+    <tableColumn id="2" name="내용" dataDxfId="4"/>
+    <tableColumn id="3" name="할당일" dataDxfId="3"/>
+    <tableColumn id="4" name="완성일" dataDxfId="2"/>
+    <tableColumn id="5" name="결과" dataDxfId="1"/>
+    <tableColumn id="6" name="문제점" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1261,23 +1327,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1297,7 +1363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="86.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="105">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1311,7 +1377,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="90">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1329,7 +1395,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="75">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -1349,7 +1415,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="103.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="120">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1369,7 +1435,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="103.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="120">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1385,7 +1451,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="224.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="240">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -1405,7 +1471,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="189.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="225">
       <c r="A8" s="1" t="s">
         <v>85</v>
       </c>
@@ -1425,7 +1491,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -1433,7 +1499,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -1441,7 +1507,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -1449,7 +1515,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -1457,7 +1523,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -1465,7 +1531,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -1473,7 +1539,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -1496,16 +1562,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="86.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="105">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -1543,7 +1609,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="120.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="135">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
@@ -1563,7 +1629,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="120.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="135">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1583,7 +1649,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -1591,7 +1657,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -1599,7 +1665,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -1607,7 +1673,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
@@ -1615,7 +1681,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -1623,7 +1689,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -1631,7 +1697,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -1639,7 +1705,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -1647,7 +1713,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -1655,7 +1721,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -1663,7 +1729,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -1686,16 +1752,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1715,7 +1781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="75">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1733,7 +1799,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="120.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="165">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1751,7 +1817,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="90">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1769,7 +1835,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="51.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="75">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -1787,7 +1853,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="103.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="105">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -1805,7 +1871,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="90">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1823,7 +1889,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="138" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="180">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1841,7 +1907,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="189.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="240">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -1861,7 +1927,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="86.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="105">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -1881,7 +1947,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="138" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="150">
       <c r="A11" s="3" t="s">
         <v>66</v>
       </c>
@@ -1901,7 +1967,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="138" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="180">
       <c r="A12" s="3" t="s">
         <v>77</v>
       </c>
@@ -1921,7 +1987,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="51.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="60">
       <c r="A13" s="1" t="s">
         <v>101</v>
       </c>
@@ -1939,7 +2005,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="75">
       <c r="A14" s="1" t="s">
         <v>103</v>
       </c>
@@ -1957,270 +2023,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="102.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43594</v>
-      </c>
-      <c r="D2" s="2">
-        <v>43594</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>43594</v>
-      </c>
-      <c r="D3" s="2">
-        <v>43594</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="114" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="6">
-        <v>43598</v>
-      </c>
-      <c r="D4" s="6">
-        <v>43598</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="2">
-        <v>43598</v>
-      </c>
-      <c r="D5" s="2">
-        <v>43598</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="71.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="2">
-        <v>43600</v>
-      </c>
-      <c r="D6" s="2">
-        <v>43600</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="117" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="2">
-        <v>43605</v>
-      </c>
-      <c r="D7" s="2">
-        <v>43606</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="74.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="2">
-        <v>43607</v>
-      </c>
-      <c r="D8" s="2">
-        <v>43607</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="142.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="2">
-        <v>42152</v>
-      </c>
-      <c r="D9" s="2">
-        <v>43614</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="2">
-        <v>42153</v>
-      </c>
-      <c r="D10" s="2">
-        <v>42153</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -2240,4 +2043,287 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G12" activeCellId="1" sqref="H11 G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="120">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43594</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43594</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="75">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43594</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43594</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="135">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="6">
+        <v>43598</v>
+      </c>
+      <c r="D4" s="6">
+        <v>43598</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="75">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43598</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43598</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105">
+      <c r="A6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43600</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43600</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="150">
+      <c r="A7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43605</v>
+      </c>
+      <c r="D7" s="2">
+        <v>43606</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="120">
+      <c r="A8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43607</v>
+      </c>
+      <c r="D8" s="2">
+        <v>43607</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="180">
+      <c r="A9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43613</v>
+      </c>
+      <c r="D9" s="2">
+        <v>43614</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="75">
+      <c r="A10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43614</v>
+      </c>
+      <c r="D10" s="2">
+        <v>42153</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="180">
+      <c r="A11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43620</v>
+      </c>
+      <c r="D11" s="2">
+        <v>43620</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="90">
+      <c r="A12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43620</v>
+      </c>
+      <c r="D12" s="2">
+        <v>43620</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>